<commit_message>
Task 13 & 14 are completed
</commit_message>
<xml_diff>
--- a/SourceCode/2023/Oct2023/Basics/SachinRawal/Task13/Test Excel.xlsx
+++ b/SourceCode/2023/Oct2023/Basics/SachinRawal/Task13/Test Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <x:si>
     <x:t>Sachin</x:t>
   </x:si>
@@ -26,6 +26,30 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">Hello </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Welcome </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">to </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">UiPath </x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Training </x:t>
+  </x:si>
+  <x:si>
+    <x:t>Session</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Column1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Column2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Column3</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -376,10 +400,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B2"/>
+  <x:dimension ref="A1:E3"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="E17" sqref="E17"/>
+      <x:selection activeCell="C4" sqref="C4"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -395,6 +419,23 @@
     <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -411,23 +452,49 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:B2"/>
+  <x:dimension ref="A1:E3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <x:c r="C1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -444,23 +511,49 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1"/>
+  <x:dimension ref="A1:B2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
-    <x:row r="1" spans="1:2">
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:2">
+      <x:c r="C1" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
         <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5">
+      <x:c r="A3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>